<commit_message>
Aggiunti valori possibili per i test di oggi
</commit_message>
<xml_diff>
--- a/Valori_compression_high.xlsx
+++ b/Valori_compression_high.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinkale/Documents/GitHub/linearVibrationsControl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\linearVibrationsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20260"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="20265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring High compression" sheetId="1" r:id="rId1"/>
     <sheet name="Spring medium compression" sheetId="2" r:id="rId2"/>
     <sheet name="Spring low compression" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>Arduino</t>
   </si>
@@ -84,7 +84,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -140,7 +140,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -151,10 +151,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0623117415322168"/>
-          <c:y val="0.0628880032060968"/>
-          <c:w val="0.892882112333001"/>
-          <c:h val="0.698034190583777"/>
+          <c:x val="6.2311741532216802E-2"/>
+          <c:y val="6.2888003206096804E-2"/>
+          <c:w val="0.89288211233300097"/>
+          <c:h val="0.69803419058377703"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -182,28 +182,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>582.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>532.0</c:v>
+                  <c:v>532</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>537.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>555.5555555555555</c:v>
+                  <c:v>555.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>550.0</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>541.6666666666667</c:v>
+                  <c:v>541.66666666666674</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>572.2222222222222</c:v>
+                  <c:v>572.22222222222217</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>562.5</c:v>
@@ -223,8 +223,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2096921984"/>
-        <c:axId val="-2096787808"/>
+        <c:axId val="1221225232"/>
+        <c:axId val="1221220336"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -266,7 +266,7 @@
                   <c:v>-0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-1.2</c:v>
@@ -292,11 +292,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2105725024"/>
-        <c:axId val="-2106588320"/>
+        <c:axId val="1221218160"/>
+        <c:axId val="1221223056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2096921984"/>
+        <c:axId val="1221225232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,10 +335,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096787808"/>
+        <c:crossAx val="1221220336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -346,7 +346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096787808"/>
+        <c:axId val="1221220336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,15 +394,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096921984"/>
+        <c:crossAx val="1221225232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2106588320"/>
+        <c:axId val="1221223056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,15 +436,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105725024"/>
+        <c:crossAx val="1221218160"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2105725024"/>
+        <c:axId val="1221218160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,7 +453,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106588320"/>
+        <c:crossAx val="1221223056"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -495,7 +496,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -525,7 +526,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1392,18 +1393,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="E10" sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>-0.13333333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2.5</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.5</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>-0.22857142857142859</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1515,7 +1516,7 @@
         <v>-0.22500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.5</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>-0.22222222222222221</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5.4</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>-0.22222222222222221</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7.2</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1599,24 +1600,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="A1:E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>